<commit_message>
material-1 data & procedure of material-2
</commit_message>
<xml_diff>
--- a/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Participant_experiment_record_sheet.xlsx
+++ b/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Participant_experiment_record_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Postgraduate\TaskRelevance\1_Study1_Task_Target\1_2_MaterialProc\1_2_2_Exp1_materials_for_experimenters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9559570-CEE7-4B56-A83D-684989869F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59624805-80FB-490B-BED1-3C2871182093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="59">
   <si>
     <t>被试序号/时间</t>
   </si>
@@ -197,6 +197,883 @@
         <family val="2"/>
       </rPr>
       <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>实验1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2560 × 1664</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>微信转账</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>预实验
+材料2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>女</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Windows</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Microsoft Edge</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>165Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_02.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测量图形和标签的匹配
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：分类重点关注朋友
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>stranger</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>self</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_03.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：区分生人的影响程度
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：分类任务只看生人图形，只看左上角标签
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1，因为目前对材料2最熟悉</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_04.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：探索对自我感知与朋友、生人之间的差异
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">： 分类任务朋友的图形，上下两个球体感觉像是朋友彼此搀扶
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料3&gt;材料2&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：对某类刺激的反应速度
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：关注生人图片
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>240Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_06.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_05.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：实验中没猜测实验目的
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">： 关注自我图形和其他的文字
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>2560 × 1600</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_07.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_08.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2560 × 1660</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1920x1080</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>144Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1920*1080</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>60Hz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测试反应能力
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">： 关注朋友（蛋），关注蛋的图像
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测试不同图形和标签的反应
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">： 朋友的图形以及标签
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料2&gt;材料3&gt;材料1</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测自我优势效应的
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">： 自我
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>记忆容易度排序：材料3&gt;材料2&gt;材料1</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -328,7 +1205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -339,32 +1216,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I6"/>
+      <selection activeCell="G32" sqref="G32:G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -663,7 +1546,7 @@
     <col min="8" max="8" width="13.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="85" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="71" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -693,105 +1576,921 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="7">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="7">
         <v>1</v>
       </c>
       <c r="G2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="8"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>2001</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6">
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="8">
         <v>25</v>
       </c>
-      <c r="I5" s="6"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="11"/>
+      <c r="G6" s="14"/>
       <c r="H6" s="9"/>
       <c r="I6" s="9"/>
     </row>
-    <row r="7" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="8">
+        <v>25</v>
+      </c>
+      <c r="I10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="9"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+    </row>
+    <row r="12" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="7">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="5">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I13" s="8"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C15" s="5">
+        <v>2002</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="8">
+        <v>25</v>
+      </c>
+      <c r="I15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="7">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" s="7">
+        <v>1</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H17" s="4">
+        <v>1</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="5">
+        <v>3</v>
+      </c>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="8"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="8"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="8"/>
+      <c r="B20" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C20" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="8">
+        <v>25</v>
+      </c>
+      <c r="I20" s="8"/>
+    </row>
+    <row r="21" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="9"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="7">
+        <v>4</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="7">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="4">
+        <v>1</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="5">
+        <v>4</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F23" s="8"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I23" s="8"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="8"/>
+      <c r="B25" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="8">
+        <v>25</v>
+      </c>
+      <c r="I25" s="8"/>
+    </row>
+    <row r="26" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="7">
+        <v>5</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="4">
+        <v>1</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="8"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I28" s="8"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="8"/>
+      <c r="B30" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C30" s="5">
+        <v>1998</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="8"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="8">
+        <v>25</v>
+      </c>
+      <c r="I30" s="8"/>
+    </row>
+    <row r="31" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="7">
+        <v>6</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F32" s="7">
+        <v>1</v>
+      </c>
+      <c r="G32" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="4">
+        <v>1</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="5">
+        <v>6</v>
+      </c>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="8"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I33" s="8"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="8"/>
+      <c r="F34" s="8"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="8"/>
+      <c r="B35" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="8">
+        <v>25</v>
+      </c>
+      <c r="I35" s="8"/>
+    </row>
+    <row r="36" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B37" s="7">
+        <v>7</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" s="7">
+        <v>1</v>
+      </c>
+      <c r="G37" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H37" s="4">
+        <v>1</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="8"/>
+      <c r="B38" s="8"/>
+      <c r="C38" s="5">
+        <v>7</v>
+      </c>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="8"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I38" s="8"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
+      <c r="C39" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="8"/>
+      <c r="B40" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C40" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="F40" s="8"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="8">
+        <v>25</v>
+      </c>
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+    </row>
+    <row r="42" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="7">
+        <v>8</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F42" s="7">
+        <v>1</v>
+      </c>
+      <c r="G42" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H42" s="4">
+        <v>1</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="5">
+        <v>8</v>
+      </c>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="F43" s="8"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" s="8"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="8"/>
+      <c r="F44" s="8"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" s="8"/>
+      <c r="B45" s="10">
+        <v>45731</v>
+      </c>
+      <c r="C45" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="8">
+        <v>25</v>
+      </c>
+      <c r="I45" s="8"/>
+    </row>
+    <row r="46" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+    </row>
+    <row r="47" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="90">
+    <mergeCell ref="I42:I46"/>
+    <mergeCell ref="E43:E45"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="A42:A46"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="G42:G46"/>
+    <mergeCell ref="I37:I41"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="H38:H39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="H40:H41"/>
+    <mergeCell ref="A37:A41"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="F37:F41"/>
+    <mergeCell ref="G37:G41"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="H33:H34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="A32:A36"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="F32:F36"/>
+    <mergeCell ref="G32:G36"/>
+    <mergeCell ref="I27:I31"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="F27:F31"/>
+    <mergeCell ref="G27:G31"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="D2:D3"/>
@@ -802,6 +2501,46 @@
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="H5:H6"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="F12:F16"/>
+    <mergeCell ref="G12:G16"/>
+    <mergeCell ref="I12:I16"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="F22:F26"/>
+    <mergeCell ref="G22:G26"/>
+    <mergeCell ref="I22:I26"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="H23:H24"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="H25:H26"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="G17:G21"/>
+    <mergeCell ref="I17:I21"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="H20:H21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add pilot version2 data & single subject data analysis
</commit_message>
<xml_diff>
--- a/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Participant_experiment_record_sheet.xlsx
+++ b/1_Study1_Task_Target/1_2_MaterialProc/1_2_2_Exp1_materials_for_experimenters/Exp1_Participant_experiment_record_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1_Postgraduate\TaskRelevance\1_Study1_Task_Target\1_2_MaterialProc\1_2_2_Exp1_materials_for_experimenters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C50308D-A1DE-4019-BC91-3FAA781D08F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F92BA504-0D85-480C-A91F-A7D2A9B56C0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="127">
   <si>
     <t>被试序号/时间</t>
   </si>
@@ -2574,6 +2574,557 @@
         <family val="2"/>
       </rPr>
       <t>：自我图形的错误数据上来看，有把自我与朋友图形记混的可能性</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预实验
+v2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>预实验
+材料2
+v1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_25.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：看图片呈现速度对反应按键的影响
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：分类任务关注自我；匹配任务关注朋友，因为更容易出错
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_26.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_27.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_28.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测量是否对自我更加敏感
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：无
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_30.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>exp1_29.csv</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测试反应力
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：两个任务都关注朋友的
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：未猜测
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：分类任务关注生人，匹配任务未特别关注
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：测量知觉加工类似的嘛？
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：没有特别关注的
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>被试是否中途退出过程序</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：否
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>是否猜测实验目的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：锻炼反应能力；记忆和匹配能力
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>有无特别关注某图形或文字</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">：朋友图形；生人图形-匹配任务
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其他</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+      </rPr>
+      <t>：</t>
     </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -2725,6 +3276,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2752,35 +3315,23 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3062,10 +3613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I157"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103:E105"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152:G156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -3109,69 +3660,69 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="14">
         <v>99</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="14">
         <v>1</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="15" t="s">
         <v>22</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="8" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="14">
+      <c r="A5" s="12"/>
+      <c r="B5" s="18">
         <v>45607</v>
       </c>
       <c r="C5" s="5">
@@ -3180,17 +3731,17 @@
       <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="8">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="12">
         <v>25</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9"/>
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
@@ -3200,75 +3751,75 @@
       <c r="E6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="14">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="14" t="s">
         <v>24</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="14">
         <v>1</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="15" t="s">
         <v>99</v>
       </c>
       <c r="H7" s="4">
         <v>1</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="12"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="8"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="14">
+      <c r="A10" s="12"/>
+      <c r="B10" s="18">
         <v>45731</v>
       </c>
       <c r="C10" s="5">
@@ -3277,17 +3828,17 @@
       <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="8">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="12">
         <v>25</v>
       </c>
-      <c r="I10" s="8"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="6" t="s">
         <v>10</v>
       </c>
@@ -3297,75 +3848,75 @@
       <c r="E11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="14">
         <v>2</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12" s="14">
         <v>1</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="G12" s="15" t="s">
         <v>100</v>
       </c>
       <c r="H12" s="4">
         <v>1</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="5">
         <v>2</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="D13" s="12"/>
+      <c r="E13" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="12"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I13" s="8"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="14">
+      <c r="A15" s="12"/>
+      <c r="B15" s="18">
         <v>45731</v>
       </c>
       <c r="C15" s="5">
@@ -3374,17 +3925,17 @@
       <c r="D15" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="8">
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="12">
         <v>25</v>
       </c>
-      <c r="I15" s="8"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9"/>
-      <c r="B16" s="9"/>
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -3394,75 +3945,75 @@
       <c r="E16" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
     </row>
     <row r="17" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="14">
         <v>3</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17" s="14">
         <v>1</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="G17" s="15" t="s">
         <v>101</v>
       </c>
       <c r="H17" s="4">
         <v>1</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="8" t="s">
+      <c r="F18" s="12"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I18" s="8"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
       <c r="C19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="14">
+      <c r="A20" s="12"/>
+      <c r="B20" s="18">
         <v>45731</v>
       </c>
       <c r="C20" s="5">
@@ -3471,17 +4022,17 @@
       <c r="D20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="8">
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="12">
         <v>25</v>
       </c>
-      <c r="I20" s="8"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
@@ -3491,75 +4042,75 @@
       <c r="E21" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="9"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="14">
         <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="14">
         <v>1</v>
       </c>
-      <c r="G22" s="11" t="s">
+      <c r="G22" s="15" t="s">
         <v>102</v>
       </c>
       <c r="H22" s="4">
         <v>1</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="5">
         <v>4</v>
       </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8" t="s">
+      <c r="D23" s="12"/>
+      <c r="E23" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="8" t="s">
+      <c r="F23" s="12"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="8"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
       <c r="C24" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="8"/>
-      <c r="B25" s="14">
+      <c r="A25" s="12"/>
+      <c r="B25" s="18">
         <v>45731</v>
       </c>
       <c r="C25" s="5">
@@ -3568,17 +4119,17 @@
       <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="8">
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="12">
         <v>25</v>
       </c>
-      <c r="I25" s="8"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="6" t="s">
         <v>10</v>
       </c>
@@ -3588,75 +4139,75 @@
       <c r="E26" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="9"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
     </row>
     <row r="27" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="14">
         <v>5</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="14">
         <v>1</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="15" t="s">
         <v>103</v>
       </c>
       <c r="H27" s="4">
         <v>1</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="5">
         <v>5</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8" t="s">
+      <c r="D28" s="12"/>
+      <c r="E28" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="F28" s="8"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="8" t="s">
+      <c r="F28" s="12"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I28" s="8"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
       <c r="C29" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="8"/>
-      <c r="B30" s="14">
+      <c r="A30" s="12"/>
+      <c r="B30" s="18">
         <v>45731</v>
       </c>
       <c r="C30" s="5">
@@ -3665,17 +4216,17 @@
       <c r="D30" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="8">
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="12">
         <v>25</v>
       </c>
-      <c r="I30" s="8"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9"/>
-      <c r="B31" s="9"/>
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
@@ -3685,75 +4236,75 @@
       <c r="E31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
     </row>
     <row r="32" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="14">
         <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="10" t="s">
+      <c r="D32" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="10">
+      <c r="F32" s="14">
         <v>1</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="15" t="s">
         <v>104</v>
       </c>
       <c r="H32" s="4">
         <v>1</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="5">
         <v>6</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8" t="s">
+      <c r="D33" s="12"/>
+      <c r="E33" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F33" s="8"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="8" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I33" s="8"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
+      <c r="A34" s="12"/>
+      <c r="B34" s="12"/>
       <c r="C34" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="8"/>
-      <c r="B35" s="14">
+      <c r="A35" s="12"/>
+      <c r="B35" s="18">
         <v>45731</v>
       </c>
       <c r="C35" s="5">
@@ -3762,17 +4313,17 @@
       <c r="D35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="8">
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="12">
         <v>25</v>
       </c>
-      <c r="I35" s="8"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
       <c r="C36" s="6" t="s">
         <v>10</v>
       </c>
@@ -3782,75 +4333,75 @@
       <c r="E36" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="9"/>
-      <c r="G36" s="13"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
     </row>
     <row r="37" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="10">
+      <c r="B37" s="14">
         <v>7</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="D37" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E37" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="10">
+      <c r="F37" s="14">
         <v>1</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="15" t="s">
         <v>105</v>
       </c>
       <c r="H37" s="4">
         <v>1</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="5">
         <v>7</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8" t="s">
+      <c r="D38" s="12"/>
+      <c r="E38" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="8"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="8" t="s">
+      <c r="F38" s="12"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I38" s="8"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
       <c r="C39" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="16"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="8"/>
-      <c r="B40" s="14">
+      <c r="A40" s="12"/>
+      <c r="B40" s="18">
         <v>45731</v>
       </c>
       <c r="C40" s="5">
@@ -3859,17 +4410,17 @@
       <c r="D40" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="8">
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="12">
         <v>25</v>
       </c>
-      <c r="I40" s="8"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
       <c r="C41" s="6" t="s">
         <v>10</v>
       </c>
@@ -3879,75 +4430,75 @@
       <c r="E41" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F41" s="9"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
+      <c r="A42" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="14">
         <v>8</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="D42" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F42" s="10">
+      <c r="F42" s="14">
         <v>1</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="15" t="s">
         <v>106</v>
       </c>
       <c r="H42" s="4">
         <v>1</v>
       </c>
-      <c r="I42" s="10" t="s">
+      <c r="I42" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="5">
         <v>8</v>
       </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8" t="s">
+      <c r="D43" s="12"/>
+      <c r="E43" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="8" t="s">
+      <c r="F43" s="12"/>
+      <c r="G43" s="16"/>
+      <c r="H43" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I43" s="8"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
       <c r="C44" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="12"/>
+      <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
-      <c r="B45" s="14">
+      <c r="A45" s="12"/>
+      <c r="B45" s="18">
         <v>45731</v>
       </c>
       <c r="C45" s="5">
@@ -3956,17 +4507,17 @@
       <c r="D45" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="8">
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="16"/>
+      <c r="H45" s="12">
         <v>25</v>
       </c>
-      <c r="I45" s="8"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
       <c r="C46" s="6" t="s">
         <v>10</v>
       </c>
@@ -3976,463 +4527,463 @@
       <c r="E46" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
     </row>
     <row r="47" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="19">
         <v>9</v>
       </c>
-      <c r="C47" s="16" t="s">
+      <c r="C47" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="15">
+      <c r="F47" s="19">
         <v>1</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G47" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="H47" s="16">
+      <c r="H47" s="7">
         <v>1</v>
       </c>
-      <c r="I47" s="15" t="s">
+      <c r="I47" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="8"/>
-      <c r="B48" s="18"/>
-      <c r="C48" s="19">
+      <c r="A48" s="12"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="8">
         <v>9</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18" t="s">
+      <c r="D48" s="20"/>
+      <c r="E48" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="F48" s="18"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="18" t="s">
+      <c r="F48" s="20"/>
+      <c r="G48" s="23"/>
+      <c r="H48" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I48" s="18"/>
+      <c r="I48" s="20"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="8"/>
-      <c r="B49" s="18"/>
-      <c r="C49" s="19" t="s">
+      <c r="A49" s="12"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E49" s="18"/>
-      <c r="F49" s="18"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="18"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="8"/>
-      <c r="B50" s="21">
+      <c r="A50" s="12"/>
+      <c r="B50" s="25">
         <v>45731</v>
       </c>
-      <c r="C50" s="19">
+      <c r="C50" s="8">
         <v>2002</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="E50" s="18"/>
-      <c r="F50" s="18"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="18">
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="20">
         <v>25</v>
       </c>
-      <c r="I50" s="18"/>
+      <c r="I50" s="20"/>
     </row>
     <row r="51" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="9"/>
-      <c r="B51" s="22"/>
-      <c r="C51" s="23" t="s">
+      <c r="A51" s="13"/>
+      <c r="B51" s="21"/>
+      <c r="C51" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D51" s="23" t="s">
+      <c r="D51" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F51" s="22"/>
+      <c r="F51" s="21"/>
       <c r="G51" s="24"/>
-      <c r="H51" s="22"/>
-      <c r="I51" s="22"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
     </row>
     <row r="52" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="19">
         <v>10</v>
       </c>
-      <c r="C52" s="16" t="s">
+      <c r="C52" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="16" t="s">
+      <c r="E52" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="15">
+      <c r="F52" s="19">
         <v>1</v>
       </c>
-      <c r="G52" s="17" t="s">
+      <c r="G52" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="H52" s="16">
+      <c r="H52" s="7">
         <v>1</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I52" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="8"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="19">
+      <c r="A53" s="12"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="8">
         <v>10</v>
       </c>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18" t="s">
+      <c r="D53" s="20"/>
+      <c r="E53" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="F53" s="18"/>
-      <c r="G53" s="20"/>
-      <c r="H53" s="18" t="s">
+      <c r="F53" s="20"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I53" s="18"/>
+      <c r="I53" s="20"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="8"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19" t="s">
+      <c r="A54" s="12"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="19" t="s">
+      <c r="D54" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="E54" s="18"/>
-      <c r="F54" s="18"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="18"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="20"/>
+      <c r="I54" s="20"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="8"/>
-      <c r="B55" s="21">
+      <c r="A55" s="12"/>
+      <c r="B55" s="25">
         <v>45732</v>
       </c>
-      <c r="C55" s="19">
+      <c r="C55" s="8">
         <v>2001</v>
       </c>
-      <c r="D55" s="25" t="s">
+      <c r="D55" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E55" s="18"/>
-      <c r="F55" s="18"/>
-      <c r="G55" s="20"/>
-      <c r="H55" s="18">
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="20">
         <v>25</v>
       </c>
-      <c r="I55" s="18"/>
+      <c r="I55" s="20"/>
     </row>
     <row r="56" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="9"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="23" t="s">
+      <c r="A56" s="13"/>
+      <c r="B56" s="21"/>
+      <c r="C56" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D56" s="23" t="s">
+      <c r="D56" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="22"/>
+      <c r="F56" s="21"/>
       <c r="G56" s="24"/>
-      <c r="H56" s="22"/>
-      <c r="I56" s="22"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
     </row>
     <row r="57" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="7" t="s">
+      <c r="A57" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B57" s="15">
+      <c r="B57" s="19">
         <v>11</v>
       </c>
-      <c r="C57" s="16" t="s">
+      <c r="C57" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F57" s="15">
+      <c r="F57" s="19">
         <v>1</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="G57" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="H57" s="16">
+      <c r="H57" s="7">
         <v>1</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I57" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="8"/>
-      <c r="B58" s="18"/>
-      <c r="C58" s="19">
+      <c r="A58" s="12"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="8">
         <v>11</v>
       </c>
-      <c r="D58" s="18"/>
-      <c r="E58" s="18" t="s">
+      <c r="D58" s="20"/>
+      <c r="E58" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="F58" s="18"/>
-      <c r="G58" s="20"/>
-      <c r="H58" s="18" t="s">
+      <c r="F58" s="20"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I58" s="18"/>
+      <c r="I58" s="20"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="8"/>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19" t="s">
+      <c r="A59" s="12"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="20"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="18"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="20"/>
+      <c r="I59" s="20"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="8"/>
-      <c r="B60" s="21">
+      <c r="A60" s="12"/>
+      <c r="B60" s="25">
         <v>45731</v>
       </c>
-      <c r="C60" s="19">
+      <c r="C60" s="8">
         <v>2000</v>
       </c>
-      <c r="D60" s="19" t="s">
+      <c r="D60" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="20"/>
-      <c r="H60" s="18">
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="23"/>
+      <c r="H60" s="20">
         <v>25</v>
       </c>
-      <c r="I60" s="18"/>
+      <c r="I60" s="20"/>
     </row>
     <row r="61" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="9"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23" t="s">
+      <c r="A61" s="13"/>
+      <c r="B61" s="21"/>
+      <c r="C61" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D61" s="23" t="s">
+      <c r="D61" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E61" s="23" t="s">
+      <c r="E61" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="22"/>
+      <c r="F61" s="21"/>
       <c r="G61" s="24"/>
-      <c r="H61" s="22"/>
-      <c r="I61" s="22"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
     </row>
     <row r="62" spans="1:9" ht="14.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="15">
+      <c r="B62" s="19">
         <v>12</v>
       </c>
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="16" t="s">
+      <c r="E62" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F62" s="15">
+      <c r="F62" s="19">
         <v>1</v>
       </c>
-      <c r="G62" s="17" t="s">
+      <c r="G62" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="H62" s="16">
+      <c r="H62" s="7">
         <v>1</v>
       </c>
-      <c r="I62" s="15" t="s">
+      <c r="I62" s="19" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="8"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="19">
+      <c r="A63" s="12"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="8">
         <v>12</v>
       </c>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18" t="s">
+      <c r="D63" s="20"/>
+      <c r="E63" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="F63" s="18"/>
-      <c r="G63" s="20"/>
-      <c r="H63" s="18" t="s">
+      <c r="F63" s="20"/>
+      <c r="G63" s="23"/>
+      <c r="H63" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="I63" s="18"/>
+      <c r="I63" s="20"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="8"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="19" t="s">
+      <c r="A64" s="12"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="E64" s="18"/>
-      <c r="F64" s="18"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="18"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="23"/>
+      <c r="H64" s="20"/>
+      <c r="I64" s="20"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="8"/>
-      <c r="B65" s="21">
+      <c r="A65" s="12"/>
+      <c r="B65" s="25">
         <v>45732</v>
       </c>
-      <c r="C65" s="19">
+      <c r="C65" s="8">
         <v>2000</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="E65" s="18"/>
-      <c r="F65" s="18"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="18">
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="23"/>
+      <c r="H65" s="20">
         <v>25</v>
       </c>
-      <c r="I65" s="18"/>
+      <c r="I65" s="20"/>
     </row>
     <row r="66" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="9"/>
-      <c r="B66" s="22"/>
-      <c r="C66" s="23" t="s">
+      <c r="A66" s="13"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D66" s="23" t="s">
+      <c r="D66" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E66" s="23" t="s">
+      <c r="E66" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="F66" s="22"/>
+      <c r="F66" s="21"/>
       <c r="G66" s="24"/>
-      <c r="H66" s="22"/>
-      <c r="I66" s="22"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
     </row>
     <row r="67" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B67" s="10">
+      <c r="B67" s="14">
         <v>13</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E67" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F67" s="10">
+      <c r="F67" s="14">
         <v>1</v>
       </c>
-      <c r="G67" s="11" t="s">
+      <c r="G67" s="15" t="s">
         <v>54</v>
       </c>
       <c r="H67" s="4">
         <v>1</v>
       </c>
-      <c r="I67" s="10" t="s">
+      <c r="I67" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
       <c r="C68" s="5">
         <v>13</v>
       </c>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8" t="s">
+      <c r="D68" s="12"/>
+      <c r="E68" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="F68" s="8"/>
-      <c r="G68" s="12"/>
-      <c r="H68" s="8" t="s">
+      <c r="F68" s="12"/>
+      <c r="G68" s="16"/>
+      <c r="H68" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I68" s="8"/>
+      <c r="I68" s="12"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
+      <c r="A69" s="12"/>
+      <c r="B69" s="12"/>
       <c r="C69" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="12"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="12"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="8"/>
-      <c r="B70" s="14">
+      <c r="A70" s="12"/>
+      <c r="B70" s="18">
         <v>45732</v>
       </c>
       <c r="C70" s="5">
@@ -4441,17 +4992,17 @@
       <c r="D70" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="12"/>
-      <c r="H70" s="8">
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="16"/>
+      <c r="H70" s="12">
         <v>25</v>
       </c>
-      <c r="I70" s="8"/>
+      <c r="I70" s="12"/>
     </row>
     <row r="71" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="9"/>
-      <c r="B71" s="9"/>
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
       <c r="C71" s="6" t="s">
         <v>10</v>
       </c>
@@ -4461,75 +5012,75 @@
       <c r="E71" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F71" s="9"/>
-      <c r="G71" s="13"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
     </row>
     <row r="72" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B72" s="10">
+      <c r="B72" s="14">
         <v>14</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="10" t="s">
+      <c r="D72" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E72" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F72" s="10">
+      <c r="F72" s="14">
         <v>1</v>
       </c>
-      <c r="G72" s="11" t="s">
+      <c r="G72" s="15" t="s">
         <v>57</v>
       </c>
       <c r="H72" s="4">
         <v>1</v>
       </c>
-      <c r="I72" s="10" t="s">
+      <c r="I72" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="8"/>
-      <c r="B73" s="8"/>
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
       <c r="C73" s="5">
         <v>14</v>
       </c>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8" t="s">
+      <c r="D73" s="12"/>
+      <c r="E73" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F73" s="8"/>
-      <c r="G73" s="12"/>
-      <c r="H73" s="8" t="s">
+      <c r="F73" s="12"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I73" s="8"/>
+      <c r="I73" s="12"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
+      <c r="A74" s="12"/>
+      <c r="B74" s="12"/>
       <c r="C74" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="12"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="16"/>
+      <c r="H74" s="12"/>
+      <c r="I74" s="12"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="8"/>
-      <c r="B75" s="14">
+      <c r="A75" s="12"/>
+      <c r="B75" s="18">
         <v>45732</v>
       </c>
       <c r="C75" s="5">
@@ -4538,17 +5089,17 @@
       <c r="D75" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="12"/>
-      <c r="H75" s="8">
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="16"/>
+      <c r="H75" s="12">
         <v>25</v>
       </c>
-      <c r="I75" s="8"/>
+      <c r="I75" s="12"/>
     </row>
     <row r="76" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="9"/>
-      <c r="B76" s="9"/>
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
       <c r="C76" s="6" t="s">
         <v>10</v>
       </c>
@@ -4558,75 +5109,75 @@
       <c r="E76" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F76" s="9"/>
-      <c r="G76" s="13"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
     </row>
     <row r="77" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B77" s="10">
+      <c r="B77" s="14">
         <v>15</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D77" s="10" t="s">
+      <c r="D77" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E77" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F77" s="10">
+      <c r="F77" s="14">
         <v>1</v>
       </c>
-      <c r="G77" s="11" t="s">
+      <c r="G77" s="15" t="s">
         <v>79</v>
       </c>
       <c r="H77" s="4">
         <v>1</v>
       </c>
-      <c r="I77" s="10" t="s">
+      <c r="I77" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
+      <c r="A78" s="12"/>
+      <c r="B78" s="12"/>
       <c r="C78" s="5">
         <v>15</v>
       </c>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8" t="s">
+      <c r="D78" s="12"/>
+      <c r="E78" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="F78" s="8"/>
-      <c r="G78" s="12"/>
-      <c r="H78" s="8" t="s">
+      <c r="F78" s="12"/>
+      <c r="G78" s="16"/>
+      <c r="H78" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I78" s="8"/>
+      <c r="I78" s="12"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
+      <c r="A79" s="12"/>
+      <c r="B79" s="12"/>
       <c r="C79" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="12"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="12"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="8"/>
-      <c r="B80" s="14">
+      <c r="A80" s="12"/>
+      <c r="B80" s="18">
         <v>45732</v>
       </c>
       <c r="C80" s="5">
@@ -4635,17 +5186,17 @@
       <c r="D80" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="12"/>
-      <c r="H80" s="8">
+      <c r="E80" s="12"/>
+      <c r="F80" s="12"/>
+      <c r="G80" s="16"/>
+      <c r="H80" s="12">
         <v>25</v>
       </c>
-      <c r="I80" s="8"/>
+      <c r="I80" s="12"/>
     </row>
     <row r="81" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
       <c r="C81" s="6" t="s">
         <v>10</v>
       </c>
@@ -4655,75 +5206,75 @@
       <c r="E81" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F81" s="9"/>
-      <c r="G81" s="13"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
     </row>
     <row r="82" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B82" s="10">
+      <c r="B82" s="14">
         <v>16</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D82" s="10" t="s">
+      <c r="D82" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E82" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F82" s="10">
+      <c r="F82" s="14">
         <v>1</v>
       </c>
-      <c r="G82" s="11" t="s">
+      <c r="G82" s="15" t="s">
         <v>111</v>
       </c>
       <c r="H82" s="4">
         <v>1</v>
       </c>
-      <c r="I82" s="10" t="s">
+      <c r="I82" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
+      <c r="A83" s="12"/>
+      <c r="B83" s="12"/>
       <c r="C83" s="5">
         <v>16</v>
       </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8" t="s">
+      <c r="D83" s="12"/>
+      <c r="E83" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="F83" s="8"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="8" t="s">
+      <c r="F83" s="12"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I83" s="8"/>
+      <c r="I83" s="12"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
+      <c r="A84" s="12"/>
+      <c r="B84" s="12"/>
       <c r="C84" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
+      <c r="E84" s="12"/>
+      <c r="F84" s="12"/>
+      <c r="G84" s="16"/>
+      <c r="H84" s="12"/>
+      <c r="I84" s="12"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="8"/>
-      <c r="B85" s="14">
+      <c r="A85" s="12"/>
+      <c r="B85" s="18">
         <v>45732</v>
       </c>
       <c r="C85" s="5">
@@ -4732,17 +5283,17 @@
       <c r="D85" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="8">
+      <c r="E85" s="12"/>
+      <c r="F85" s="12"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="12">
         <v>25</v>
       </c>
-      <c r="I85" s="8"/>
+      <c r="I85" s="12"/>
     </row>
     <row r="86" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A86" s="9"/>
-      <c r="B86" s="9"/>
+      <c r="A86" s="13"/>
+      <c r="B86" s="13"/>
       <c r="C86" s="6" t="s">
         <v>10</v>
       </c>
@@ -4752,75 +5303,75 @@
       <c r="E86" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F86" s="9"/>
-      <c r="G86" s="13"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
     </row>
     <row r="87" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B87" s="10">
+      <c r="B87" s="14">
         <v>17</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D87" s="10" t="s">
+      <c r="D87" s="14" t="s">
         <v>30</v>
       </c>
       <c r="E87" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F87" s="10">
+      <c r="F87" s="14">
         <v>1</v>
       </c>
-      <c r="G87" s="11" t="s">
+      <c r="G87" s="15" t="s">
         <v>63</v>
       </c>
       <c r="H87" s="4">
         <v>1</v>
       </c>
-      <c r="I87" s="10" t="s">
+      <c r="I87" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
+      <c r="A88" s="12"/>
+      <c r="B88" s="12"/>
       <c r="C88" s="5">
         <v>17</v>
       </c>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8" t="s">
+      <c r="D88" s="12"/>
+      <c r="E88" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="F88" s="8"/>
-      <c r="G88" s="12"/>
-      <c r="H88" s="8" t="s">
+      <c r="F88" s="12"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I88" s="8"/>
+      <c r="I88" s="12"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
+      <c r="A89" s="12"/>
+      <c r="B89" s="12"/>
       <c r="C89" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="12"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
+      <c r="E89" s="12"/>
+      <c r="F89" s="12"/>
+      <c r="G89" s="16"/>
+      <c r="H89" s="12"/>
+      <c r="I89" s="12"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="8"/>
-      <c r="B90" s="14">
+      <c r="A90" s="12"/>
+      <c r="B90" s="18">
         <v>45732</v>
       </c>
       <c r="C90" s="5">
@@ -4829,17 +5380,17 @@
       <c r="D90" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E90" s="8"/>
-      <c r="F90" s="8"/>
-      <c r="G90" s="12"/>
-      <c r="H90" s="8">
+      <c r="E90" s="12"/>
+      <c r="F90" s="12"/>
+      <c r="G90" s="16"/>
+      <c r="H90" s="12">
         <v>25</v>
       </c>
-      <c r="I90" s="8"/>
+      <c r="I90" s="12"/>
     </row>
     <row r="91" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="6" t="s">
         <v>10</v>
       </c>
@@ -4849,75 +5400,75 @@
       <c r="E91" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F91" s="9"/>
-      <c r="G91" s="13"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="9"/>
+      <c r="F91" s="13"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="13"/>
+      <c r="I91" s="13"/>
     </row>
     <row r="92" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B92" s="10">
+      <c r="B92" s="14">
         <v>18</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D92" s="10" t="s">
+      <c r="D92" s="14" t="s">
         <v>58</v>
       </c>
       <c r="E92" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F92" s="10">
+      <c r="F92" s="14">
         <v>1</v>
       </c>
-      <c r="G92" s="11" t="s">
+      <c r="G92" s="15" t="s">
         <v>64</v>
       </c>
       <c r="H92" s="4">
         <v>1</v>
       </c>
-      <c r="I92" s="10" t="s">
+      <c r="I92" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
+      <c r="A93" s="12"/>
+      <c r="B93" s="12"/>
       <c r="C93" s="5">
         <v>18</v>
       </c>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8" t="s">
+      <c r="D93" s="12"/>
+      <c r="E93" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="F93" s="8"/>
-      <c r="G93" s="12"/>
-      <c r="H93" s="8" t="s">
+      <c r="F93" s="12"/>
+      <c r="G93" s="16"/>
+      <c r="H93" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I93" s="8"/>
+      <c r="I93" s="12"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
+      <c r="A94" s="12"/>
+      <c r="B94" s="12"/>
       <c r="C94" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="12"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
+      <c r="E94" s="12"/>
+      <c r="F94" s="12"/>
+      <c r="G94" s="16"/>
+      <c r="H94" s="12"/>
+      <c r="I94" s="12"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="8"/>
-      <c r="B95" s="14">
+      <c r="A95" s="12"/>
+      <c r="B95" s="18">
         <v>45732</v>
       </c>
       <c r="C95" s="5">
@@ -4926,17 +5477,17 @@
       <c r="D95" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="12"/>
-      <c r="H95" s="8">
+      <c r="E95" s="12"/>
+      <c r="F95" s="12"/>
+      <c r="G95" s="16"/>
+      <c r="H95" s="12">
         <v>25</v>
       </c>
-      <c r="I95" s="8"/>
+      <c r="I95" s="12"/>
     </row>
     <row r="96" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="9"/>
-      <c r="B96" s="9"/>
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
       <c r="C96" s="6" t="s">
         <v>10</v>
       </c>
@@ -4946,75 +5497,75 @@
       <c r="E96" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F96" s="9"/>
-      <c r="G96" s="13"/>
-      <c r="H96" s="9"/>
-      <c r="I96" s="9"/>
+      <c r="F96" s="13"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="13"/>
+      <c r="I96" s="13"/>
     </row>
     <row r="97" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="7" t="s">
+      <c r="A97" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B97" s="10">
+      <c r="B97" s="14">
         <v>19</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D97" s="10" t="s">
+      <c r="D97" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E97" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F97" s="10">
+      <c r="F97" s="14">
         <v>1</v>
       </c>
-      <c r="G97" s="11" t="s">
+      <c r="G97" s="15" t="s">
         <v>70</v>
       </c>
       <c r="H97" s="4">
         <v>1</v>
       </c>
-      <c r="I97" s="10" t="s">
+      <c r="I97" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
+      <c r="A98" s="12"/>
+      <c r="B98" s="12"/>
       <c r="C98" s="5">
         <v>19</v>
       </c>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8" t="s">
+      <c r="D98" s="12"/>
+      <c r="E98" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="F98" s="8"/>
-      <c r="G98" s="12"/>
-      <c r="H98" s="8" t="s">
+      <c r="F98" s="12"/>
+      <c r="G98" s="16"/>
+      <c r="H98" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I98" s="8"/>
+      <c r="I98" s="12"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="8"/>
-      <c r="B99" s="8"/>
+      <c r="A99" s="12"/>
+      <c r="B99" s="12"/>
       <c r="C99" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E99" s="8"/>
-      <c r="F99" s="8"/>
-      <c r="G99" s="12"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="8"/>
+      <c r="E99" s="12"/>
+      <c r="F99" s="12"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="12"/>
+      <c r="I99" s="12"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="8"/>
-      <c r="B100" s="14">
+      <c r="A100" s="12"/>
+      <c r="B100" s="18">
         <v>45732</v>
       </c>
       <c r="C100" s="5">
@@ -5023,17 +5574,17 @@
       <c r="D100" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="12"/>
-      <c r="H100" s="8">
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="12">
         <v>25</v>
       </c>
-      <c r="I100" s="8"/>
+      <c r="I100" s="12"/>
     </row>
     <row r="101" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="9"/>
-      <c r="B101" s="9"/>
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
       <c r="C101" s="6" t="s">
         <v>10</v>
       </c>
@@ -5043,75 +5594,75 @@
       <c r="E101" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F101" s="9"/>
-      <c r="G101" s="13"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
+      <c r="F101" s="13"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="13"/>
+      <c r="I101" s="13"/>
     </row>
     <row r="102" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B102" s="10">
+      <c r="B102" s="14">
         <v>20</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D102" s="10" t="s">
+      <c r="D102" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E102" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F102" s="10">
+      <c r="F102" s="14">
         <v>1</v>
       </c>
-      <c r="G102" s="11" t="s">
+      <c r="G102" s="15" t="s">
         <v>71</v>
       </c>
       <c r="H102" s="4">
         <v>1</v>
       </c>
-      <c r="I102" s="10" t="s">
+      <c r="I102" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="8"/>
-      <c r="B103" s="8"/>
+      <c r="A103" s="12"/>
+      <c r="B103" s="12"/>
       <c r="C103" s="5">
         <v>20</v>
       </c>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8" t="s">
+      <c r="D103" s="12"/>
+      <c r="E103" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="F103" s="8"/>
-      <c r="G103" s="12"/>
-      <c r="H103" s="8" t="s">
+      <c r="F103" s="12"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I103" s="8"/>
+      <c r="I103" s="12"/>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="8"/>
-      <c r="B104" s="8"/>
+      <c r="A104" s="12"/>
+      <c r="B104" s="12"/>
       <c r="C104" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="12"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="8"/>
+      <c r="E104" s="12"/>
+      <c r="F104" s="12"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="12"/>
+      <c r="I104" s="12"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="8"/>
-      <c r="B105" s="14">
+      <c r="A105" s="12"/>
+      <c r="B105" s="18">
         <v>45732</v>
       </c>
       <c r="C105" s="5">
@@ -5120,17 +5671,17 @@
       <c r="D105" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="12"/>
-      <c r="H105" s="8">
+      <c r="E105" s="12"/>
+      <c r="F105" s="12"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="12">
         <v>25</v>
       </c>
-      <c r="I105" s="8"/>
+      <c r="I105" s="12"/>
     </row>
     <row r="106" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A106" s="9"/>
-      <c r="B106" s="9"/>
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
       <c r="C106" s="6" t="s">
         <v>10</v>
       </c>
@@ -5140,75 +5691,75 @@
       <c r="E106" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="F106" s="9"/>
-      <c r="G106" s="13"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
+      <c r="F106" s="13"/>
+      <c r="G106" s="17"/>
+      <c r="H106" s="13"/>
+      <c r="I106" s="13"/>
     </row>
     <row r="107" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="7" t="s">
+      <c r="A107" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B107" s="10">
+      <c r="B107" s="14">
         <v>21</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D107" s="10" t="s">
+      <c r="D107" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E107" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F107" s="10">
+      <c r="F107" s="14">
         <v>1</v>
       </c>
-      <c r="G107" s="11" t="s">
+      <c r="G107" s="15" t="s">
         <v>74</v>
       </c>
       <c r="H107" s="4">
         <v>1</v>
       </c>
-      <c r="I107" s="10" t="s">
+      <c r="I107" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="8"/>
-      <c r="B108" s="8"/>
+      <c r="A108" s="12"/>
+      <c r="B108" s="12"/>
       <c r="C108" s="5">
         <v>21</v>
       </c>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8" t="s">
+      <c r="D108" s="12"/>
+      <c r="E108" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="F108" s="8"/>
-      <c r="G108" s="12"/>
-      <c r="H108" s="8" t="s">
+      <c r="F108" s="12"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I108" s="8"/>
+      <c r="I108" s="12"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="8"/>
-      <c r="B109" s="8"/>
+      <c r="A109" s="12"/>
+      <c r="B109" s="12"/>
       <c r="C109" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="12"/>
-      <c r="H109" s="8"/>
-      <c r="I109" s="8"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="12"/>
+      <c r="I109" s="12"/>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="8"/>
-      <c r="B110" s="14">
+      <c r="A110" s="12"/>
+      <c r="B110" s="18">
         <v>45732</v>
       </c>
       <c r="C110" s="5">
@@ -5217,17 +5768,17 @@
       <c r="D110" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="12"/>
-      <c r="H110" s="8">
+      <c r="E110" s="12"/>
+      <c r="F110" s="12"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="12">
         <v>25</v>
       </c>
-      <c r="I110" s="8"/>
+      <c r="I110" s="12"/>
     </row>
     <row r="111" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A111" s="9"/>
-      <c r="B111" s="9"/>
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
       <c r="C111" s="6" t="s">
         <v>10</v>
       </c>
@@ -5237,75 +5788,75 @@
       <c r="E111" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F111" s="9"/>
-      <c r="G111" s="13"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
+      <c r="F111" s="13"/>
+      <c r="G111" s="17"/>
+      <c r="H111" s="13"/>
+      <c r="I111" s="13"/>
     </row>
     <row r="112" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="7" t="s">
+      <c r="A112" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B112" s="10">
+      <c r="B112" s="14">
         <v>22</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D112" s="10" t="s">
+      <c r="D112" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E112" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F112" s="10">
+      <c r="F112" s="14">
         <v>1</v>
       </c>
-      <c r="G112" s="11" t="s">
+      <c r="G112" s="15" t="s">
         <v>76</v>
       </c>
       <c r="H112" s="4">
         <v>1</v>
       </c>
-      <c r="I112" s="10" t="s">
+      <c r="I112" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
       <c r="C113" s="5">
         <v>22</v>
       </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8" t="s">
+      <c r="D113" s="12"/>
+      <c r="E113" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="F113" s="8"/>
-      <c r="G113" s="12"/>
-      <c r="H113" s="8" t="s">
+      <c r="F113" s="12"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I113" s="8"/>
+      <c r="I113" s="12"/>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
       <c r="C114" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="12"/>
-      <c r="H114" s="8"/>
-      <c r="I114" s="8"/>
+      <c r="E114" s="12"/>
+      <c r="F114" s="12"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="12"/>
+      <c r="I114" s="12"/>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="8"/>
-      <c r="B115" s="14">
+      <c r="A115" s="12"/>
+      <c r="B115" s="18">
         <v>45732</v>
       </c>
       <c r="C115" s="5">
@@ -5314,17 +5865,17 @@
       <c r="D115" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="12"/>
-      <c r="H115" s="8">
+      <c r="E115" s="12"/>
+      <c r="F115" s="12"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="12">
         <v>25</v>
       </c>
-      <c r="I115" s="8"/>
+      <c r="I115" s="12"/>
     </row>
     <row r="116" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A116" s="9"/>
-      <c r="B116" s="9"/>
+      <c r="A116" s="13"/>
+      <c r="B116" s="13"/>
       <c r="C116" s="6" t="s">
         <v>10</v>
       </c>
@@ -5334,75 +5885,75 @@
       <c r="E116" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F116" s="9"/>
-      <c r="G116" s="13"/>
-      <c r="H116" s="9"/>
-      <c r="I116" s="9"/>
+      <c r="F116" s="13"/>
+      <c r="G116" s="17"/>
+      <c r="H116" s="13"/>
+      <c r="I116" s="13"/>
     </row>
     <row r="117" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="7" t="s">
+      <c r="A117" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B117" s="10">
+      <c r="B117" s="14">
         <v>23</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D117" s="10" t="s">
+      <c r="D117" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F117" s="10">
+      <c r="F117" s="14">
         <v>1</v>
       </c>
-      <c r="G117" s="11" t="s">
+      <c r="G117" s="15" t="s">
         <v>77</v>
       </c>
       <c r="H117" s="4">
         <v>1</v>
       </c>
-      <c r="I117" s="10" t="s">
+      <c r="I117" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="8"/>
-      <c r="B118" s="8"/>
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
       <c r="C118" s="5">
         <v>23</v>
       </c>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8" t="s">
+      <c r="D118" s="12"/>
+      <c r="E118" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F118" s="8"/>
-      <c r="G118" s="12"/>
-      <c r="H118" s="8" t="s">
+      <c r="F118" s="12"/>
+      <c r="G118" s="16"/>
+      <c r="H118" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I118" s="8"/>
+      <c r="I118" s="12"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
       <c r="C119" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="12"/>
-      <c r="H119" s="8"/>
-      <c r="I119" s="8"/>
+      <c r="E119" s="12"/>
+      <c r="F119" s="12"/>
+      <c r="G119" s="16"/>
+      <c r="H119" s="12"/>
+      <c r="I119" s="12"/>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="8"/>
-      <c r="B120" s="14">
+      <c r="A120" s="12"/>
+      <c r="B120" s="18">
         <v>45732</v>
       </c>
       <c r="C120" s="5">
@@ -5411,17 +5962,17 @@
       <c r="D120" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="12"/>
-      <c r="H120" s="8">
+      <c r="E120" s="12"/>
+      <c r="F120" s="12"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="12">
         <v>25</v>
       </c>
-      <c r="I120" s="8"/>
+      <c r="I120" s="12"/>
     </row>
     <row r="121" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="9"/>
-      <c r="B121" s="9"/>
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
       <c r="C121" s="6" t="s">
         <v>10</v>
       </c>
@@ -5431,75 +5982,75 @@
       <c r="E121" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F121" s="9"/>
-      <c r="G121" s="13"/>
-      <c r="H121" s="9"/>
-      <c r="I121" s="9"/>
+      <c r="F121" s="13"/>
+      <c r="G121" s="17"/>
+      <c r="H121" s="13"/>
+      <c r="I121" s="13"/>
     </row>
     <row r="122" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B122" s="10">
+      <c r="A122" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122" s="14">
         <v>24</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D122" s="10" t="s">
+      <c r="D122" s="14" t="s">
         <v>65</v>
       </c>
       <c r="E122" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F122" s="10">
+      <c r="F122" s="14">
         <v>1</v>
       </c>
-      <c r="G122" s="11" t="s">
+      <c r="G122" s="15" t="s">
         <v>112</v>
       </c>
       <c r="H122" s="4">
         <v>1</v>
       </c>
-      <c r="I122" s="10" t="s">
+      <c r="I122" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
+      <c r="A123" s="12"/>
+      <c r="B123" s="12"/>
       <c r="C123" s="5">
         <v>24</v>
       </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8" t="s">
+      <c r="D123" s="12"/>
+      <c r="E123" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="F123" s="8"/>
-      <c r="G123" s="12"/>
-      <c r="H123" s="8" t="s">
+      <c r="F123" s="12"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I123" s="8"/>
+      <c r="I123" s="12"/>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="8"/>
-      <c r="B124" s="8"/>
+      <c r="A124" s="12"/>
+      <c r="B124" s="12"/>
       <c r="C124" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="12"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
+      <c r="E124" s="12"/>
+      <c r="F124" s="12"/>
+      <c r="G124" s="16"/>
+      <c r="H124" s="12"/>
+      <c r="I124" s="12"/>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="8"/>
-      <c r="B125" s="14">
+      <c r="A125" s="12"/>
+      <c r="B125" s="18">
         <v>45732</v>
       </c>
       <c r="C125" s="5">
@@ -5508,17 +6059,17 @@
       <c r="D125" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E125" s="8"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="12"/>
-      <c r="H125" s="8">
+      <c r="E125" s="12"/>
+      <c r="F125" s="12"/>
+      <c r="G125" s="16"/>
+      <c r="H125" s="12">
         <v>25</v>
       </c>
-      <c r="I125" s="8"/>
+      <c r="I125" s="12"/>
     </row>
     <row r="126" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A126" s="9"/>
-      <c r="B126" s="9"/>
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
       <c r="C126" s="6" t="s">
         <v>10</v>
       </c>
@@ -5528,14 +6079,592 @@
       <c r="E126" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F126" s="9"/>
-      <c r="G126" s="13"/>
-      <c r="H126" s="9"/>
-      <c r="I126" s="9"/>
-    </row>
-    <row r="127" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
+      <c r="F126" s="13"/>
+      <c r="G126" s="17"/>
+      <c r="H126" s="13"/>
+      <c r="I126" s="13"/>
+    </row>
+    <row r="127" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B127" s="14">
+        <v>25</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D127" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E127" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F127" s="14">
+        <v>1</v>
+      </c>
+      <c r="G127" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H127" s="4">
+        <v>0</v>
+      </c>
+      <c r="I127" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12"/>
+      <c r="C128" s="5">
+        <v>25</v>
+      </c>
+      <c r="D128" s="12"/>
+      <c r="E128" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="F128" s="12"/>
+      <c r="G128" s="16"/>
+      <c r="H128" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I128" s="12"/>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A129" s="12"/>
+      <c r="B129" s="12"/>
+      <c r="C129" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D129" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E129" s="12"/>
+      <c r="F129" s="12"/>
+      <c r="G129" s="16"/>
+      <c r="H129" s="12"/>
+      <c r="I129" s="12"/>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A130" s="12"/>
+      <c r="B130" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C130" s="5">
+        <v>2004</v>
+      </c>
+      <c r="D130" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E130" s="12"/>
+      <c r="F130" s="12"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="12">
+        <v>25</v>
+      </c>
+      <c r="I130" s="12"/>
+    </row>
+    <row r="131" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F131" s="13"/>
+      <c r="G131" s="17"/>
+      <c r="H131" s="13"/>
+      <c r="I131" s="13"/>
+    </row>
+    <row r="132" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B132" s="14">
+        <v>26</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E132" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F132" s="14">
+        <v>1</v>
+      </c>
+      <c r="G132" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H132" s="4">
+        <v>0</v>
+      </c>
+      <c r="I132" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A133" s="12"/>
+      <c r="B133" s="12"/>
+      <c r="C133" s="5">
+        <v>26</v>
+      </c>
+      <c r="D133" s="12"/>
+      <c r="E133" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F133" s="12"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I133" s="12"/>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A134" s="12"/>
+      <c r="B134" s="12"/>
+      <c r="C134" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E134" s="12"/>
+      <c r="F134" s="12"/>
+      <c r="G134" s="16"/>
+      <c r="H134" s="12"/>
+      <c r="I134" s="12"/>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A135" s="12"/>
+      <c r="B135" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C135" s="5">
+        <v>2002</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E135" s="12"/>
+      <c r="F135" s="12"/>
+      <c r="G135" s="16"/>
+      <c r="H135" s="12">
+        <v>25</v>
+      </c>
+      <c r="I135" s="12"/>
+    </row>
+    <row r="136" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E136" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F136" s="13"/>
+      <c r="G136" s="17"/>
+      <c r="H136" s="13"/>
+      <c r="I136" s="13"/>
+    </row>
+    <row r="137" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B137" s="14">
+        <v>27</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D137" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F137" s="14">
+        <v>1</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="H137" s="4">
+        <v>0</v>
+      </c>
+      <c r="I137" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A138" s="12"/>
+      <c r="B138" s="12"/>
+      <c r="C138" s="5">
+        <v>27</v>
+      </c>
+      <c r="D138" s="12"/>
+      <c r="E138" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F138" s="12"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I138" s="12"/>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A139" s="12"/>
+      <c r="B139" s="12"/>
+      <c r="C139" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E139" s="12"/>
+      <c r="F139" s="12"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="12"/>
+      <c r="I139" s="12"/>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A140" s="12"/>
+      <c r="B140" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C140" s="5"/>
+      <c r="D140" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E140" s="12"/>
+      <c r="F140" s="12"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="12">
+        <v>25</v>
+      </c>
+      <c r="I140" s="12"/>
+    </row>
+    <row r="141" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="13"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E141" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F141" s="13"/>
+      <c r="G141" s="17"/>
+      <c r="H141" s="13"/>
+      <c r="I141" s="13"/>
+    </row>
+    <row r="142" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B142" s="14">
+        <v>28</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D142" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F142" s="14">
+        <v>1</v>
+      </c>
+      <c r="G142" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H142" s="4">
+        <v>0</v>
+      </c>
+      <c r="I142" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A143" s="12"/>
+      <c r="B143" s="12"/>
+      <c r="C143" s="5">
+        <v>27</v>
+      </c>
+      <c r="D143" s="12"/>
+      <c r="E143" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F143" s="12"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I143" s="12"/>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A144" s="12"/>
+      <c r="B144" s="12"/>
+      <c r="C144" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E144" s="12"/>
+      <c r="F144" s="12"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="12"/>
+      <c r="I144" s="12"/>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A145" s="12"/>
+      <c r="B145" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C145" s="5">
+        <v>2002</v>
+      </c>
+      <c r="D145" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E145" s="12"/>
+      <c r="F145" s="12"/>
+      <c r="G145" s="16"/>
+      <c r="H145" s="12">
+        <v>25</v>
+      </c>
+      <c r="I145" s="12"/>
+    </row>
+    <row r="146" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A146" s="13"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E146" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F146" s="13"/>
+      <c r="G146" s="17"/>
+      <c r="H146" s="13"/>
+      <c r="I146" s="13"/>
+    </row>
+    <row r="147" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A147" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B147" s="14">
+        <v>29</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D147" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E147" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F147" s="14">
+        <v>1</v>
+      </c>
+      <c r="G147" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="H147" s="4">
+        <v>0</v>
+      </c>
+      <c r="I147" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A148" s="12"/>
+      <c r="B148" s="12"/>
+      <c r="C148" s="5">
+        <v>27</v>
+      </c>
+      <c r="D148" s="12"/>
+      <c r="E148" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F148" s="12"/>
+      <c r="G148" s="16"/>
+      <c r="H148" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I148" s="12"/>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A149" s="12"/>
+      <c r="B149" s="12"/>
+      <c r="C149" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D149" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E149" s="12"/>
+      <c r="F149" s="12"/>
+      <c r="G149" s="16"/>
+      <c r="H149" s="12"/>
+      <c r="I149" s="12"/>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A150" s="12"/>
+      <c r="B150" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C150" s="5"/>
+      <c r="D150" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E150" s="12"/>
+      <c r="F150" s="12"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="12">
+        <v>25</v>
+      </c>
+      <c r="I150" s="12"/>
+    </row>
+    <row r="151" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A151" s="13"/>
+      <c r="B151" s="13"/>
+      <c r="C151" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E151" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F151" s="13"/>
+      <c r="G151" s="17"/>
+      <c r="H151" s="13"/>
+      <c r="I151" s="13"/>
+    </row>
+    <row r="152" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B152" s="14">
+        <v>30</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D152" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E152" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F152" s="14">
+        <v>1</v>
+      </c>
+      <c r="G152" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="H152" s="4">
+        <v>0</v>
+      </c>
+      <c r="I152" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A153" s="12"/>
+      <c r="B153" s="12"/>
+      <c r="C153" s="5">
+        <v>30</v>
+      </c>
+      <c r="D153" s="12"/>
+      <c r="E153" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F153" s="12"/>
+      <c r="G153" s="16"/>
+      <c r="H153" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I153" s="12"/>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A154" s="12"/>
+      <c r="B154" s="12"/>
+      <c r="C154" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E154" s="12"/>
+      <c r="F154" s="12"/>
+      <c r="G154" s="16"/>
+      <c r="H154" s="12"/>
+      <c r="I154" s="12"/>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A155" s="12"/>
+      <c r="B155" s="18">
+        <v>45740</v>
+      </c>
+      <c r="C155" s="5">
+        <v>2001</v>
+      </c>
+      <c r="D155" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E155" s="12"/>
+      <c r="F155" s="12"/>
+      <c r="G155" s="16"/>
+      <c r="H155" s="12">
+        <v>25</v>
+      </c>
+      <c r="I155" s="12"/>
+    </row>
+    <row r="156" spans="1:9" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A156" s="13"/>
+      <c r="B156" s="13"/>
+      <c r="C156" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E156" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F156" s="13"/>
+      <c r="G156" s="17"/>
+      <c r="H156" s="13"/>
+      <c r="I156" s="13"/>
+    </row>
+    <row r="157" spans="1:9" ht="14.5" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="250">
+  <mergeCells count="310">
     <mergeCell ref="A62:A66"/>
     <mergeCell ref="B62:B64"/>
     <mergeCell ref="D62:D63"/>
@@ -5786,6 +6915,66 @@
     <mergeCell ref="H123:H124"/>
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="H125:H126"/>
+    <mergeCell ref="A127:A131"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="D127:D128"/>
+    <mergeCell ref="F127:F131"/>
+    <mergeCell ref="G127:G131"/>
+    <mergeCell ref="I127:I131"/>
+    <mergeCell ref="E128:E130"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="H130:H131"/>
+    <mergeCell ref="A132:A136"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="D132:D133"/>
+    <mergeCell ref="F132:F136"/>
+    <mergeCell ref="G132:G136"/>
+    <mergeCell ref="I132:I136"/>
+    <mergeCell ref="E133:E135"/>
+    <mergeCell ref="H133:H134"/>
+    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="H135:H136"/>
+    <mergeCell ref="A142:A146"/>
+    <mergeCell ref="B142:B144"/>
+    <mergeCell ref="D142:D143"/>
+    <mergeCell ref="F142:F146"/>
+    <mergeCell ref="G142:G146"/>
+    <mergeCell ref="I142:I146"/>
+    <mergeCell ref="E143:E145"/>
+    <mergeCell ref="H143:H144"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="H145:H146"/>
+    <mergeCell ref="A137:A141"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="D137:D138"/>
+    <mergeCell ref="F137:F141"/>
+    <mergeCell ref="G137:G141"/>
+    <mergeCell ref="I137:I141"/>
+    <mergeCell ref="E138:E140"/>
+    <mergeCell ref="H138:H139"/>
+    <mergeCell ref="B140:B141"/>
+    <mergeCell ref="H140:H141"/>
+    <mergeCell ref="A147:A151"/>
+    <mergeCell ref="B147:B149"/>
+    <mergeCell ref="D147:D148"/>
+    <mergeCell ref="F147:F151"/>
+    <mergeCell ref="G147:G151"/>
+    <mergeCell ref="I147:I151"/>
+    <mergeCell ref="E148:E150"/>
+    <mergeCell ref="H148:H149"/>
+    <mergeCell ref="B150:B151"/>
+    <mergeCell ref="H150:H151"/>
+    <mergeCell ref="A152:A156"/>
+    <mergeCell ref="B152:B154"/>
+    <mergeCell ref="D152:D153"/>
+    <mergeCell ref="F152:F156"/>
+    <mergeCell ref="G152:G156"/>
+    <mergeCell ref="I152:I156"/>
+    <mergeCell ref="E153:E155"/>
+    <mergeCell ref="H153:H154"/>
+    <mergeCell ref="B155:B156"/>
+    <mergeCell ref="H155:H156"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>